<commit_message>
skip non exist stuff
</commit_message>
<xml_diff>
--- a/sampledata/sampleTransferNoWellIds.xlsx
+++ b/sampledata/sampleTransferNoWellIds.xlsx
@@ -69,9 +69,6 @@
     <t>A5</t>
   </si>
   <si>
-    <t>A7</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -81,10 +78,13 @@
     <t>A8</t>
   </si>
   <si>
-    <t>ssdest000000141jul17_C</t>
-  </si>
-  <si>
-    <t>ssdest000000141jul17_384_C</t>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul17_D</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul17_384_D</t>
   </si>
 </sst>
 </file>
@@ -154,8 +154,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -228,7 +232,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -257,6 +261,8 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +291,8 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,7 +676,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -731,7 +739,7 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -740,7 +748,7 @@
         <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -749,7 +757,7 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
removed unused columns from spreadsheet
</commit_message>
<xml_diff>
--- a/sampledata/sampleTransferNoWellIds.xlsx
+++ b/sampledata/sampleTransferNoWellIds.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,35 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Source Plate Barcode</t>
   </si>
   <si>
-    <t>Source Well Id</t>
-  </si>
-  <si>
-    <t>Source Col/Row</t>
-  </si>
-  <si>
-    <t>Destination Plate Type</t>
-  </si>
-  <si>
-    <t>Destination Well Id</t>
-  </si>
-  <si>
-    <t>Destination Col/Row</t>
-  </si>
-  <si>
     <t>Destination Plate Barcode</t>
   </si>
   <si>
-    <t>96 well, plastic</t>
-  </si>
-  <si>
-    <t>384 well, plastic</t>
-  </si>
-  <si>
     <t>ssdest000000141jul15</t>
   </si>
   <si>
@@ -81,13 +60,19 @@
     <t>A6</t>
   </si>
   <si>
-    <t>ssdest000000141jul17_E</t>
-  </si>
-  <si>
-    <t>ssdest000000141jul17_384_E</t>
-  </si>
-  <si>
     <t>Dest Well Count</t>
+  </si>
+  <si>
+    <t>Source Well</t>
+  </si>
+  <si>
+    <t>Destination Well</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul17_G</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul17_384_G</t>
   </si>
 </sst>
 </file>
@@ -157,8 +142,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -245,7 +238,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -281,6 +274,10 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -316,6 +313,10 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,172 +646,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35" customHeight="1">
+    <row r="1" spans="1:5" ht="35" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="E4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7">
+      <c r="E7">
         <v>384</v>
       </c>
     </row>

</xml_diff>